<commit_message>
generated a few more tables and figures
</commit_message>
<xml_diff>
--- a/Qualitative_work/Qualitative_consultations/3_Paper/3_Findings_Tables_&_Graphs.xlsx
+++ b/Qualitative_work/Qualitative_consultations/3_Paper/3_Findings_Tables_&_Graphs.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/l_nabwire_cgiar_org/Documents/L.Nabwire/git/Maize_Uganda/mippi_UG/Qualitative_work/Qualitative_consultations/3_Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{079C2CC4-E505-4595-8BF2-E046D0304603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77EA1B3D-9D04-48D0-913C-9B04E5BA1B2F}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{079C2CC4-E505-4595-8BF2-E046D0304603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6A53EC0-8536-4680-A459-2389E49E17B2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="q1" sheetId="14" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <pivotCache cacheId="2" r:id="rId13"/>
     <pivotCache cacheId="3" r:id="rId14"/>
     <pivotCache cacheId="4" r:id="rId15"/>
+    <pivotCache cacheId="9" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="193">
   <si>
     <t>Aroma</t>
   </si>
@@ -625,6 +626,9 @@
   </si>
   <si>
     <t>Why the maize consumption-related traits are important?</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1181,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1273,6 +1277,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1318,7 +1323,55 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="28">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.00000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0000000000"/>
+    </dxf>
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -1678,6 +1731,417 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[3_Findings_Tables_&amp;_Graphs.xlsx]q3!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'q3'!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'q3'!$F$4:$F$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Alcohol brew</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fries/snacks</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Boiled maize</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Roasted maize</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Porridge</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Posho</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'q3'!$G$4:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.2631578947368416</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0175438596491224</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.526315789473683</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.543859649122805</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.82456140350877</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.82456140350877</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8526-4672-BABD-6853E2B41EBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="853083664"/>
+        <c:axId val="853085824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="853083664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="853085824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="853085824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Proportion (%) of responses </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="853083664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2145,7 +2609,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2637,7 +3101,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3264,6 +3728,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4271,7 +4775,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4475,6 +4979,509 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -4775,7 +5782,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5326,6 +6333,47 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>139699</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7391A915-B95E-4DAD-728C-29110400A431}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>1114425</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>409575</xdr:rowOff>
@@ -5362,7 +6410,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5403,7 +6451,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5653,6 +6701,37 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Administrator" refreshedDate="45045.927777777775" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="17" xr:uid="{3E382416-3F4A-4B68-BF24-7520DCAF1AA9}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B3:D20" sheet="q3"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Dishes" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Posho"/>
+        <s v="Porridge"/>
+        <s v="Roasted maize"/>
+        <s v="Fries/snacks"/>
+        <s v="Boiled maize"/>
+        <s v="Alcohol brew"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number of respondents in the group" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="4"/>
+    </cacheField>
+    <cacheField name="Proportion (%) of responses" numFmtId="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.5087719298245612" maxValue="7.0175438596491224"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="47">
   <r>
@@ -6419,6 +7498,96 @@
     <s v="."/>
     <n v="3"/>
     <n v="8.5714285714285712"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="17">
+  <r>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="5.2631578947368416"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="5.2631578947368416"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="3"/>
+    <n v="5.2631578947368416"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2"/>
+    <n v="3.5087719298245612"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="3.5087719298245612"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="3.5087719298245612"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2"/>
+    <n v="3.5087719298245612"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -6516,16 +7685,16 @@
     <dataField name="Sum of Proportion (%) of responses" fld="3" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="11">
+    <format dxfId="27">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="26">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="25">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="24">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -6542,6 +7711,103 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E675071-7F9E-4464-9AE0-05F19B533BF5}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+  <location ref="F3:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="6">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="2" outline="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Proportion (%) of responses" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EBADF12C-F5D6-4898-80AD-826B5D8825DD}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="H4:I10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
@@ -6598,13 +7864,13 @@
     <dataField name="Sum of Proportion (%) of responses" fld="3" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="7">
+    <format dxfId="23">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="22">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="21">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -6631,7 +7897,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43900DDE-4AE8-4A74-9C83-721BACE09DFD}" name="PivotTable13" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="J3:K22" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
@@ -6761,7 +8027,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD7B56AD-6965-4F2A-A066-26CE81EAEFCC}" name="PivotTable12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="G3:H14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
@@ -6838,14 +8104,14 @@
     <dataField name="Sum of Proportion (%) of responses" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="4">
+    <format dxfId="20">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="19">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -6881,7 +8147,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C166D0B-B9FC-4007-A373-7A63ACD9AB31}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="G3:H9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
@@ -6938,21 +8204,21 @@
     <dataField name="Sum of Proportion (%) of responses" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="2">
+    <format dxfId="18">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="17">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="16">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -9057,10 +10323,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9068,220 +10334,349 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7265625" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>80</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7">
+        <v>4</v>
+      </c>
+      <c r="D4" s="24">
+        <f>(C4/$C$21)*$D$1</f>
+        <v>7.0175438596491224</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="24">
+        <v>5.2631578947368416</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" s="24">
+        <f t="shared" ref="D5:D20" si="0">(C5/$C$21)*$D$1</f>
+        <v>7.0175438596491224</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="24">
+        <v>7.0175438596491224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" s="24">
+        <f t="shared" si="0"/>
+        <v>7.0175438596491224</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="24">
+        <v>10.526315789473683</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>110</v>
       </c>
       <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7">
         <v>4</v>
       </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" s="24">
+        <f t="shared" si="0"/>
+        <v>7.0175438596491224</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="24">
+        <v>17.543859649122805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" s="24">
+        <f t="shared" si="0"/>
+        <v>7.0175438596491224</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="24">
+        <v>29.82456140350877</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="7">
+        <v>4</v>
+      </c>
+      <c r="D9" s="24">
+        <f t="shared" si="0"/>
+        <v>7.0175438596491224</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="24">
+        <v>29.82456140350877</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" s="24">
+        <f t="shared" si="0"/>
+        <v>7.0175438596491224</v>
+      </c>
+      <c r="F10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" s="24">
+        <f t="shared" si="0"/>
+        <v>7.0175438596491224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7">
+        <v>4</v>
+      </c>
+      <c r="D12" s="24">
+        <f t="shared" si="0"/>
+        <v>7.0175438596491224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C12">
+      <c r="C13" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" s="24">
+        <f t="shared" si="0"/>
+        <v>7.0175438596491224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" s="24">
+        <f t="shared" si="0"/>
+        <v>5.2631578947368416</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7">
+        <v>3</v>
+      </c>
+      <c r="D15" s="24">
+        <f t="shared" si="0"/>
+        <v>5.2631578947368416</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="24">
+        <f t="shared" si="0"/>
+        <v>5.2631578947368416</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="C17" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="24">
+        <f t="shared" si="0"/>
+        <v>3.5087719298245612</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" s="24">
+        <f t="shared" si="0"/>
+        <v>3.5087719298245612</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>14</v>
       </c>
       <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2</v>
+      </c>
+      <c r="D19" s="24">
+        <f t="shared" si="0"/>
+        <v>3.5087719298245612</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="C19">
+      <c r="C20" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C20">
-        <f>SUM(C3:C19)</f>
+      <c r="D20" s="24">
+        <f t="shared" si="0"/>
+        <v>3.5087719298245612</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <f>SUM(C4:C20)</f>
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -11852,7 +13247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0333135-A200-4502-A2AF-55EFCFC926D5}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Did a bit of formatting on the graphs and tables to export to lyx
</commit_message>
<xml_diff>
--- a/Qualitative_work/Qualitative_consultations/3_Paper/3_Findings_Tables_&_Graphs.xlsx
+++ b/Qualitative_work/Qualitative_consultations/3_Paper/3_Findings_Tables_&_Graphs.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/l_nabwire_cgiar_org/Documents/L.Nabwire/git/Maize_Uganda/mippi_UG/Qualitative_work/Qualitative_consultations/3_Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{079C2CC4-E505-4595-8BF2-E046D0304603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6A53EC0-8536-4680-A459-2389E49E17B2}"/>
+  <xr:revisionPtr revIDLastSave="294" documentId="13_ncr:1_{079C2CC4-E505-4595-8BF2-E046D0304603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27C6E802-8DB7-471A-8583-569F7BBC66FC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="q1" sheetId="14" r:id="rId1"/>
@@ -20,18 +20,19 @@
     <sheet name="q5" sheetId="30" r:id="rId5"/>
     <sheet name="q6" sheetId="8" r:id="rId6"/>
     <sheet name="q7" sheetId="28" r:id="rId7"/>
-    <sheet name="7a" sheetId="23" r:id="rId8"/>
-    <sheet name="q8" sheetId="31" r:id="rId9"/>
-    <sheet name="q9" sheetId="32" r:id="rId10"/>
+    <sheet name="q7_" sheetId="34" r:id="rId8"/>
+    <sheet name="7a" sheetId="23" r:id="rId9"/>
+    <sheet name="q8" sheetId="31" r:id="rId10"/>
+    <sheet name="q9" sheetId="32" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId11"/>
-    <pivotCache cacheId="1" r:id="rId12"/>
-    <pivotCache cacheId="2" r:id="rId13"/>
-    <pivotCache cacheId="3" r:id="rId14"/>
-    <pivotCache cacheId="4" r:id="rId15"/>
-    <pivotCache cacheId="9" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId12"/>
+    <pivotCache cacheId="1" r:id="rId13"/>
+    <pivotCache cacheId="6" r:id="rId14"/>
+    <pivotCache cacheId="3" r:id="rId15"/>
+    <pivotCache cacheId="4" r:id="rId16"/>
+    <pivotCache cacheId="5" r:id="rId17"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="203">
   <si>
     <t>Aroma</t>
   </si>
@@ -629,6 +630,36 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>\\</t>
+  </si>
+  <si>
+    <t>why is the trait considered important</t>
+  </si>
+  <si>
+    <t>Good taste gives appetite; Good taste keeps you satisfied longer; Sweet for the mouth</t>
+  </si>
+  <si>
+    <t>Feeds more people; More food to feed many people; You need less flour to make a big meal</t>
+  </si>
+  <si>
+    <t>Takes a short time; Takes less firewood/charcoal</t>
+  </si>
+  <si>
+    <t>Takes less firewood; Takes less water to prepare</t>
+  </si>
+  <si>
+    <t>Percent of responses</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1308,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1323,54 +1354,18 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="16">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.0000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000000000"/>
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
@@ -1547,13 +1542,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>44.230769230769226</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.948717948717949</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.820512820512819</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2127,8 +2122,6 @@
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -2159,73 +2152,15 @@
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" b="1"/>
-              <a:t>Ways</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-              <a:t> in which maize consumers identify and differentiate between varieties</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -2300,7 +2235,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2595,8 +2532,6 @@
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -2623,569 +2558,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[3_Findings_Tables_&amp;_Graphs.xlsx]q7!PivotTable12</c:name>
-    <c:fmtId val="1"/>
+    <c:name>[3_Findings_Tables_&amp;_Graphs.xlsx]q8!PivotTable2</c:name>
+    <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" b="1"/>
-              <a:t>Traits that consumers consider most important when consuming maize and maize products</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'q7'!$H$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'q7'!$G$4:$G$14</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>Aroma</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Nutrition/protein</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Ease of cooking</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Fine flour texture</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Milling out-turn</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Grain coating</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Cooking time</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Color (whiter grain/flour)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Flour expansion after cooking</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Grain size/weight</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Palatability (sweet and smooth taste)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'q7'!$H$4:$H$14</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1.7391304347826086</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7391304347826086</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.2173913043478262</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.2173913043478262</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.2173913043478262</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.2173913043478262</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.0869565217391308</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.304347826086957</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13.913043478260869</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14.782608695652174</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>29.565217391304351</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D20B-45F0-804F-EA34DFBA0FAF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="451012920"/>
-        <c:axId val="451013280"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="451012920"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="451013280"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="451013280"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Proportion of responses</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="451012920"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst>
-    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
-      <c14:pivotOptions>
-        <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZonesVisible val="1"/>
-      </c14:pivotOptions>
-    </c:ext>
-    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
-      <c16:pivotOptions16>
-        <c16:showExpandCollapseFieldButtons val="1"/>
-      </c16:pivotOptions16>
-    </c:ext>
-  </c:extLst>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:pivotSource>
-    <c:name>[3_Findings_Tables_&amp;_Graphs.xlsx]q8!PivotTable2</c:name>
-    <c:fmtId val="0"/>
-  </c:pivotSource>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>A</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> good maize variety for consumption is one that:</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -3260,7 +2645,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3554,8 +2941,6 @@
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -3689,46 +3074,6 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5782,511 +5127,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6411,47 +5251,6 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>12699</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2033B0DD-133E-EF17-A90B-3D2A95923F3E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7594,7 +6393,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1EB29193-974F-472C-88A7-4CC1BDC915E4}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="G3:I18" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <location ref="G3:H18" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="3">
@@ -7622,7 +6421,7 @@
       </items>
     </pivotField>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="2" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="2" outline="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
     <field x="0"/>
@@ -7681,20 +6480,17 @@
   <colItems count="1">
     <i/>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Proportion (%) of responses" fld="3" baseField="0" baseItem="0" numFmtId="2"/>
-  </dataFields>
   <formats count="4">
-    <format dxfId="27">
+    <format dxfId="15">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="14">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="13">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="12">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -7711,7 +6507,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E675071-7F9E-4464-9AE0-05F19B533BF5}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E675071-7F9E-4464-9AE0-05F19B533BF5}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="14">
   <location ref="F3:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -7769,14 +6565,14 @@
     <dataField name="Sum of Proportion (%) of responses" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="8">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
@@ -7808,7 +6604,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EBADF12C-F5D6-4898-80AD-826B5D8825DD}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EBADF12C-F5D6-4898-80AD-826B5D8825DD}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="10">
   <location ref="H4:I10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -7864,13 +6660,13 @@
     <dataField name="Sum of Proportion (%) of responses" fld="3" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="23">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="10">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="9">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -7898,7 +6694,127 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43900DDE-4AE8-4A74-9C83-721BACE09DFD}" name="PivotTable13" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD7B56AD-6965-4F2A-A066-26CE81EAEFCC}" name="PivotTable12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+  <location ref="G3:H14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="8"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="5"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="2" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Proportion (%) of responses" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43900DDE-4AE8-4A74-9C83-721BACE09DFD}" name="PivotTable13" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="J3:K22" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -8027,128 +6943,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD7B56AD-6965-4F2A-A066-26CE81EAEFCC}" name="PivotTable12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
-  <location ref="G3:H14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending">
-      <items count="12">
-        <item x="8"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="10"/>
-        <item x="5"/>
-        <item x="9"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="2" outline="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Proportion (%) of responses" fld="2" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="20">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="19">
-      <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C166D0B-B9FC-4007-A373-7A63ACD9AB31}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C166D0B-B9FC-4007-A373-7A63ACD9AB31}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="4">
   <location ref="G3:H9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -8204,21 +7000,21 @@
     <dataField name="Sum of Proportion (%) of responses" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="18">
+    <format dxfId="6">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="4">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -8542,13 +7338,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="K23" sqref="K23:N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8563,11 +7359,12 @@
     <col min="8" max="8" width="30.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6328125" customWidth="1"/>
     <col min="10" max="10" width="4.36328125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" customWidth="1"/>
+    <col min="11" max="11" width="30.1796875" customWidth="1"/>
+    <col min="12" max="12" width="8.26953125" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>25</v>
       </c>
@@ -8576,7 +7373,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -8586,7 +7383,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
@@ -8609,18 +7406,19 @@
       <c r="H3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="26" t="s">
-        <v>185</v>
-      </c>
+      <c r="I3"/>
       <c r="J3" s="31"/>
       <c r="K3" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="L3" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M3" s="28" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -8643,15 +7441,18 @@
       <c r="H4" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="24">
-        <v>1.2820512820512819</v>
-      </c>
       <c r="K4" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L4" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -8671,17 +7472,20 @@
       <c r="H5" t="s">
         <v>144</v>
       </c>
-      <c r="I5" s="24">
-        <v>11.538461538461538</v>
-      </c>
       <c r="K5" t="s">
         <v>144</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M5" s="24">
         <v>11.538461538461538</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -8701,17 +7505,20 @@
       <c r="H6" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="24">
-        <v>2.5641025641025639</v>
-      </c>
       <c r="K6" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L6" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M6" s="24">
         <v>10.256410256410255</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -8731,17 +7538,20 @@
       <c r="H7" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="24">
-        <v>10.256410256410255</v>
-      </c>
       <c r="K7" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="24">
+      <c r="L7" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M7" s="24">
         <v>7.6923076923076925</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -8761,17 +7571,20 @@
       <c r="H8" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="24">
-        <v>1.2820512820512819</v>
-      </c>
       <c r="K8" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="24">
+      <c r="L8" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M8" s="24">
         <v>4.4871794871794872</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -8791,17 +7604,20 @@
       <c r="H9" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="24">
-        <v>7.6923076923076925</v>
-      </c>
       <c r="K9" t="s">
         <v>31</v>
       </c>
-      <c r="L9" s="24">
+      <c r="L9" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M9" s="24">
         <v>3.8461538461538458</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -8821,17 +7637,20 @@
       <c r="H10" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="24">
-        <v>4.4871794871794872</v>
-      </c>
       <c r="K10" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="24">
+      <c r="L10" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M10" s="24">
         <v>2.5641025641025639</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -8851,17 +7670,20 @@
       <c r="H11" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="24">
-        <v>3.8461538461538458</v>
-      </c>
       <c r="K11" t="s">
         <v>39</v>
       </c>
-      <c r="L11" s="24">
+      <c r="L11" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M11" s="24">
         <v>1.2820512820512819</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -8884,17 +7706,20 @@
       <c r="H12" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="24">
-        <v>4.4871794871794872</v>
-      </c>
       <c r="K12" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="24">
+      <c r="L12" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M12" s="24">
         <v>1.2820512820512819</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -8914,12 +7739,21 @@
       <c r="H13" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="24">
-        <v>10.897435897435896</v>
-      </c>
-      <c r="L13" s="24"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L13" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M13" s="24">
+        <f>SUM(M5:M12)</f>
+        <v>42.948717948717956</v>
+      </c>
+      <c r="N13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -8939,15 +7773,18 @@
       <c r="H14" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="24">
-        <v>8.3333333333333321</v>
-      </c>
       <c r="K14" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="L14" s="24"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L14" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M14" s="24"/>
+      <c r="N14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -8967,17 +7804,20 @@
       <c r="H15" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="24">
-        <v>1.2820512820512819</v>
-      </c>
       <c r="K15" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="24">
+      <c r="L15" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M15" s="24">
         <v>14.102564102564102</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -8997,17 +7837,20 @@
       <c r="H16" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="24">
-        <v>5.1282051282051277</v>
-      </c>
       <c r="K16" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="24">
+      <c r="L16" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M16" s="24">
         <v>10.897435897435896</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -9027,17 +7870,20 @@
       <c r="H17" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="24">
-        <v>14.102564102564102</v>
-      </c>
       <c r="K17" t="s">
         <v>30</v>
       </c>
-      <c r="L17" s="24">
+      <c r="L17" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M17" s="24">
         <v>8.3333333333333321</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -9060,17 +7906,20 @@
       <c r="H18" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="24">
-        <v>12.820512820512819</v>
-      </c>
       <c r="K18" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="24">
+      <c r="L18" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M18" s="24">
         <v>5.1282051282051277</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -9090,11 +7939,17 @@
       <c r="K19" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="24">
+      <c r="L19" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M19" s="24">
         <v>4.4871794871794872</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -9117,11 +7972,17 @@
       <c r="K20" t="s">
         <v>34</v>
       </c>
-      <c r="L20" s="24">
+      <c r="L20" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M20" s="24">
         <v>1.2820512820512819</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -9143,11 +8004,23 @@
       </c>
       <c r="H21" s="23">
         <f>SUM(I12:I17)</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L21" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M21" s="24">
+        <f>SUM(M15:M20)</f>
         <v>44.230769230769226</v>
       </c>
-      <c r="L21" s="24"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N21" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -9169,14 +8042,20 @@
       </c>
       <c r="H22" s="23">
         <f>SUM(I4:I11)</f>
-        <v>42.948717948717949</v>
+        <v>0</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="L22" s="24"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L22" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M22" s="24"/>
+      <c r="N22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -9196,18 +8075,24 @@
       <c r="G23" t="s">
         <v>183</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="23" t="e">
         <f>GETPIVOTDATA("Proportion (%) of responses",$G$3,"Attribute category","Production &amp; consumption","attribute","Maturity time")</f>
-        <v>12.820512820512819</v>
+        <v>#REF!</v>
       </c>
       <c r="K23" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="L23" s="30">
+      <c r="L23" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M23" s="30">
         <v>12.820512820512819</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N23" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -9224,8 +8109,21 @@
         <f t="shared" si="0"/>
         <v>1.2820512820512819</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K24" s="41" t="s">
+        <v>193</v>
+      </c>
+      <c r="L24" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M24" s="24">
+        <f>SUM(M23)</f>
+        <v>12.820512820512819</v>
+      </c>
+      <c r="N24" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -9243,7 +8141,7 @@
         <v>1.2820512820512819</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -9261,7 +8159,7 @@
         <v>1.2820512820512819</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -9279,7 +8177,7 @@
         <v>1.2820512820512819</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -9297,7 +8195,7 @@
         <v>1.2820512820512819</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -9315,7 +8213,7 @@
         <v>1.2820512820512819</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -9333,7 +8231,7 @@
         <v>1.2820512820512819</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -9351,7 +8249,7 @@
         <v>1.2820512820512819</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -9714,6 +8612,289 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0333135-A200-4502-A2AF-55EFCFC926D5}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.26953125" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="7" max="7" width="45.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3</v>
+      </c>
+      <c r="E4" s="24">
+        <f>(D4/$D$14)*$E$1</f>
+        <v>8.5714285714285712</v>
+      </c>
+      <c r="G4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H4" s="24">
+        <v>8.5714285714285712</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+      <c r="E5" s="24">
+        <f t="shared" ref="E5:E13" si="0">(D5/$D$14)*$E$1</f>
+        <v>8.5714285714285712</v>
+      </c>
+      <c r="G5" t="s">
+        <v>164</v>
+      </c>
+      <c r="H5" s="24">
+        <v>8.5714285714285712</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="7">
+        <v>3</v>
+      </c>
+      <c r="E6" s="24">
+        <f t="shared" si="0"/>
+        <v>8.5714285714285712</v>
+      </c>
+      <c r="G6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H6" s="24">
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4</v>
+      </c>
+      <c r="E7" s="24">
+        <f t="shared" si="0"/>
+        <v>11.428571428571429</v>
+      </c>
+      <c r="G7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" s="24">
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4</v>
+      </c>
+      <c r="E8" s="24">
+        <f t="shared" si="0"/>
+        <v>11.428571428571429</v>
+      </c>
+      <c r="G8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8" s="24">
+        <v>28.571428571428569</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4</v>
+      </c>
+      <c r="E9" s="24">
+        <f t="shared" si="0"/>
+        <v>11.428571428571429</v>
+      </c>
+      <c r="G9" t="s">
+        <v>170</v>
+      </c>
+      <c r="H9" s="24">
+        <v>31.428571428571431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4</v>
+      </c>
+      <c r="E10" s="24">
+        <f t="shared" si="0"/>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="7">
+        <v>4</v>
+      </c>
+      <c r="E11" s="24">
+        <f t="shared" si="0"/>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="7">
+        <v>3</v>
+      </c>
+      <c r="E12" s="24">
+        <f t="shared" si="0"/>
+        <v>8.5714285714285712</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="7">
+        <v>3</v>
+      </c>
+      <c r="E13" s="24">
+        <f t="shared" si="0"/>
+        <v>8.5714285714285712</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D14" s="36">
+        <f>SUM(D4:D13)</f>
+        <v>35</v>
+      </c>
+      <c r="E14" s="36">
+        <f>SUM(E4:E13)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE09B661-4CCA-41F3-A565-4309240B90AC}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -10325,8 +9506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10513,7 +9694,7 @@
       <c r="F10" t="s">
         <v>192</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G10">
         <v>100</v>
       </c>
     </row>
@@ -11050,7 +10231,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11464,10 +10645,10 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12447,11 +11628,281 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
-  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFECC893-9DC8-4F98-A754-8DFA5B5BA96D}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.36328125" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.36328125" customWidth="1"/>
+    <col min="5" max="5" width="78.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="24">
+        <v>29.565217391304351</v>
+      </c>
+      <c r="D2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="24">
+        <v>14.782608695652174</v>
+      </c>
+      <c r="D3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" s="24">
+        <v>13.913043478260869</v>
+      </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="24">
+        <v>11.304347826086957</v>
+      </c>
+      <c r="D5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" s="24">
+        <v>6.0869565217391308</v>
+      </c>
+      <c r="D6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="24">
+        <v>5.2173913043478262</v>
+      </c>
+      <c r="D7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="24">
+        <v>5.2173913043478262</v>
+      </c>
+      <c r="D8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" t="s">
+        <v>202</v>
+      </c>
+      <c r="F8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="24">
+        <v>5.2173913043478262</v>
+      </c>
+      <c r="D9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" s="24">
+        <v>5.2173913043478262</v>
+      </c>
+      <c r="D10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" s="24">
+        <v>1.7391304347826086</v>
+      </c>
+      <c r="D11" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>194</v>
+      </c>
+      <c r="C12" s="24">
+        <v>1.7391304347826086</v>
+      </c>
+      <c r="D12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
+    <sortCondition descending="1" ref="C2:C12"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="F1" r:id="rId1" xr:uid="{23A77438-92D4-457D-9A79-DCABFC1E3A86}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{36AFC6C0-8CC7-4E71-9E7E-15D562A308EC}"/>
+    <hyperlink ref="F3:F12" r:id="rId3" display="\\" xr:uid="{36A3B0C4-989F-4A72-BD05-CE208A32A965}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BDF51F-BA95-4FAF-84C4-1C25E40F6E58}">
   <dimension ref="A1:E70"/>
   <sheetViews>
@@ -13241,287 +12692,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0333135-A200-4502-A2AF-55EFCFC926D5}">
-  <dimension ref="A1:I14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="7" max="7" width="45.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="E1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="7">
-        <v>3</v>
-      </c>
-      <c r="E4" s="24">
-        <f>(D4/$D$14)*$E$1</f>
-        <v>8.5714285714285712</v>
-      </c>
-      <c r="G4" t="s">
-        <v>167</v>
-      </c>
-      <c r="H4" s="24">
-        <v>8.5714285714285712</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="7">
-        <v>3</v>
-      </c>
-      <c r="E5" s="24">
-        <f t="shared" ref="E5:E13" si="0">(D5/$D$14)*$E$1</f>
-        <v>8.5714285714285712</v>
-      </c>
-      <c r="G5" t="s">
-        <v>164</v>
-      </c>
-      <c r="H5" s="24">
-        <v>8.5714285714285712</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" t="s">
-        <v>167</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="7">
-        <v>3</v>
-      </c>
-      <c r="E6" s="24">
-        <f t="shared" si="0"/>
-        <v>8.5714285714285712</v>
-      </c>
-      <c r="G6" t="s">
-        <v>168</v>
-      </c>
-      <c r="H6" s="24">
-        <v>11.428571428571429</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="7">
-        <v>4</v>
-      </c>
-      <c r="E7" s="24">
-        <f t="shared" si="0"/>
-        <v>11.428571428571429</v>
-      </c>
-      <c r="G7" t="s">
-        <v>169</v>
-      </c>
-      <c r="H7" s="24">
-        <v>11.428571428571429</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="7">
-        <v>4</v>
-      </c>
-      <c r="E8" s="24">
-        <f t="shared" si="0"/>
-        <v>11.428571428571429</v>
-      </c>
-      <c r="G8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H8" s="24">
-        <v>28.571428571428569</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" t="s">
-        <v>168</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="7">
-        <v>4</v>
-      </c>
-      <c r="E9" s="24">
-        <f t="shared" si="0"/>
-        <v>11.428571428571429</v>
-      </c>
-      <c r="G9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H9" s="24">
-        <v>31.428571428571431</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>170</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="7">
-        <v>4</v>
-      </c>
-      <c r="E10" s="24">
-        <f t="shared" si="0"/>
-        <v>11.428571428571429</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>169</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="7">
-        <v>4</v>
-      </c>
-      <c r="E11" s="24">
-        <f t="shared" si="0"/>
-        <v>11.428571428571429</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="7">
-        <v>3</v>
-      </c>
-      <c r="E12" s="24">
-        <f t="shared" si="0"/>
-        <v>8.5714285714285712</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="7">
-        <v>3</v>
-      </c>
-      <c r="E13" s="24">
-        <f t="shared" si="0"/>
-        <v>8.5714285714285712</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D14" s="36">
-        <f>SUM(D4:D13)</f>
-        <v>35</v>
-      </c>
-      <c r="E14" s="36">
-        <f>SUM(E4:E13)</f>
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
-  <drawing r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
minor formatting on sheet 7
</commit_message>
<xml_diff>
--- a/Qualitative_work/Qualitative_consultations/3_Paper/3_Findings_Tables_&_Graphs.xlsx
+++ b/Qualitative_work/Qualitative_consultations/3_Paper/3_Findings_Tables_&_Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/l_nabwire_cgiar_org/Documents/L.Nabwire/git/Maize_Uganda/mippi_UG/Qualitative_work/Qualitative_consultations/3_Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="294" documentId="13_ncr:1_{079C2CC4-E505-4595-8BF2-E046D0304603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27C6E802-8DB7-471A-8583-569F7BBC66FC}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="13_ncr:1_{079C2CC4-E505-4595-8BF2-E046D0304603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{294722D8-521F-4B43-8FD1-2E139BC4966C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="q1" sheetId="14" r:id="rId1"/>
@@ -29,7 +29,7 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId12"/>
     <pivotCache cacheId="1" r:id="rId13"/>
-    <pivotCache cacheId="6" r:id="rId14"/>
+    <pivotCache cacheId="2" r:id="rId14"/>
     <pivotCache cacheId="3" r:id="rId15"/>
     <pivotCache cacheId="4" r:id="rId16"/>
     <pivotCache cacheId="5" r:id="rId17"/>
@@ -1212,7 +1212,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1308,7 +1308,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1354,19 +1353,7 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -1384,6 +1371,12 @@
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
@@ -2558,6 +2551,388 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
+    <c:name>[3_Findings_Tables_&amp;_Graphs.xlsx]q7!PivotTable12</c:name>
+    <c:fmtId val="2"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'q7'!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'q7'!$G$4:$G$14</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Aroma</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nutrition/protein</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ease of cooking</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fine flour texture</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Milling out-turn</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Grain coating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Cooking time</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Color (whiter grain/flour)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Flour expansion after cooking</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Grain size/weight</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Palatability (sweet and smooth taste)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'q7'!$H$4:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.7391304347826086</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7391304347826086</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2173913043478262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2173913043478262</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2173913043478262</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.2173913043478262</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0869565217391308</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.304347826086957</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.913043478260869</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.782608695652174</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29.565217391304351</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-63D4-437C-8108-4013285776FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="571885968"/>
+        <c:axId val="571887408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="571885968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="571887408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="571887408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="571885968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
     <c:name>[3_Findings_Tables_&amp;_Graphs.xlsx]q8!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
@@ -3113,6 +3488,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4623,6 +5038,511 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5251,6 +6171,47 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1987550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{902C5097-78F4-15D3-C70F-019126D32D8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6481,16 +7442,16 @@
     <i/>
   </colItems>
   <formats count="4">
-    <format dxfId="15">
+    <format dxfId="13">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="12">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="13">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="10">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -6565,14 +7526,14 @@
     <dataField name="Sum of Proportion (%) of responses" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="2">
+    <format dxfId="9">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="8">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
@@ -6660,13 +7621,13 @@
     <dataField name="Sum of Proportion (%) of responses" fld="3" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="11">
+    <format dxfId="7">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="5">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -6694,7 +7655,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD7B56AD-6965-4F2A-A066-26CE81EAEFCC}" name="PivotTable12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD7B56AD-6965-4F2A-A066-26CE81EAEFCC}" name="PivotTable12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
   <location ref="G3:H14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending">
@@ -6770,18 +7731,18 @@
     <dataField name="Sum of Proportion (%) of responses" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="8">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="3">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="2">
+  <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -6792,6 +7753,15 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -6814,7 +7784,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43900DDE-4AE8-4A74-9C83-721BACE09DFD}" name="PivotTable13" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43900DDE-4AE8-4A74-9C83-721BACE09DFD}" name="PivotTable13" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="J3:K22" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -7000,21 +7970,21 @@
     <dataField name="Sum of Proportion (%) of responses" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="6">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="0">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -7341,10 +8311,10 @@
   <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K23" sqref="K23:N24"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8109,7 +9079,7 @@
         <f t="shared" si="0"/>
         <v>1.2820512820512819</v>
       </c>
-      <c r="K24" s="41" t="s">
+      <c r="K24" s="2" t="s">
         <v>193</v>
       </c>
       <c r="L24" s="27" t="s">
@@ -8615,7 +9585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0333135-A200-4502-A2AF-55EFCFC926D5}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -10644,11 +11614,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E8F723-8302-46E0-80A7-A4B507221238}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11628,6 +12598,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
made a few figure and text edits
</commit_message>
<xml_diff>
--- a/Qualitative_work/Qualitative_consultations/3_Paper/3_Findings_Tables_&_Graphs.xlsx
+++ b/Qualitative_work/Qualitative_consultations/3_Paper/3_Findings_Tables_&_Graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/l_nabwire_cgiar_org/Documents/L.Nabwire/git/Maize_Uganda/mippi_UG/Qualitative_work/Qualitative_consultations/3_Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="13_ncr:1_{079C2CC4-E505-4595-8BF2-E046D0304603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{294722D8-521F-4B43-8FD1-2E139BC4966C}"/>
+  <xr:revisionPtr revIDLastSave="521" documentId="13_ncr:1_{079C2CC4-E505-4595-8BF2-E046D0304603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD5C9F7A-C34F-466C-B86E-4F463BA5CAFE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="q1" sheetId="14" r:id="rId1"/>
@@ -24,15 +24,16 @@
     <sheet name="7a" sheetId="23" r:id="rId9"/>
     <sheet name="q8" sheetId="31" r:id="rId10"/>
     <sheet name="q9" sheetId="32" r:id="rId11"/>
+    <sheet name="Number consulted" sheetId="35" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId12"/>
-    <pivotCache cacheId="1" r:id="rId13"/>
-    <pivotCache cacheId="2" r:id="rId14"/>
-    <pivotCache cacheId="3" r:id="rId15"/>
-    <pivotCache cacheId="4" r:id="rId16"/>
-    <pivotCache cacheId="5" r:id="rId17"/>
+    <pivotCache cacheId="0" r:id="rId13"/>
+    <pivotCache cacheId="1" r:id="rId14"/>
+    <pivotCache cacheId="2" r:id="rId15"/>
+    <pivotCache cacheId="3" r:id="rId16"/>
+    <pivotCache cacheId="4" r:id="rId17"/>
+    <pivotCache cacheId="5" r:id="rId18"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="223">
   <si>
     <t>Aroma</t>
   </si>
@@ -593,18 +594,6 @@
     <t>Fine flour texture</t>
   </si>
   <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>Consuption-related traits</t>
-  </si>
-  <si>
-    <t>Production-related traits</t>
-  </si>
-  <si>
-    <t>Both production &amp; consumption traits</t>
-  </si>
-  <si>
     <t>Proportion (%) of responses</t>
   </si>
   <si>
@@ -644,22 +633,94 @@
     <t>why is the trait considered important</t>
   </si>
   <si>
-    <t>Good taste gives appetite; Good taste keeps you satisfied longer; Sweet for the mouth</t>
-  </si>
-  <si>
-    <t>Feeds more people; More food to feed many people; You need less flour to make a big meal</t>
-  </si>
-  <si>
-    <t>Takes a short time; Takes less firewood/charcoal</t>
-  </si>
-  <si>
-    <t>Takes less firewood; Takes less water to prepare</t>
-  </si>
-  <si>
     <t>Percent of responses</t>
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Category of maize consumer</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Number consulted</t>
+  </si>
+  <si>
+    <t>Maize seed dealers</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>Maize farmers</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Maize Millers</t>
+  </si>
+  <si>
+    <t>Maize traders</t>
+  </si>
+  <si>
+    <t>Total men</t>
+  </si>
+  <si>
+    <t>Total women</t>
+  </si>
+  <si>
+    <t>District Agricultural Technical and research staff</t>
+  </si>
+  <si>
+    <t>Good taste gives appetite.</t>
+  </si>
+  <si>
+    <t>Good taste keeps you satisfied longer.</t>
+  </si>
+  <si>
+    <t>Sweet for the mouth.</t>
+  </si>
+  <si>
+    <t>Gives more flour.</t>
+  </si>
+  <si>
+    <t>Feeds more people.</t>
+  </si>
+  <si>
+    <t>More food to feed many people.</t>
+  </si>
+  <si>
+    <t>You need less flour to make a big meal.</t>
+  </si>
+  <si>
+    <t>Takes a short time; Takes less firewood/charcoal.</t>
+  </si>
+  <si>
+    <t>Takes less firewood.</t>
+  </si>
+  <si>
+    <t>Takes less water to prepare.</t>
+  </si>
+  <si>
+    <t>Big grain coat is good for roasted maize, but produces a low milling out-turn.</t>
+  </si>
+  <si>
+    <t>Aroma provides appetite.</t>
+  </si>
+  <si>
+    <t>provides energy.</t>
+  </si>
+  <si>
+    <t>Consumption Total</t>
+  </si>
+  <si>
+    <t>Production Total</t>
+  </si>
+  <si>
+    <t>Production &amp; consumption Total</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1093,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1167,6 +1228,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1212,7 +1288,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1296,6 +1372,20 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1353,7 +1443,7 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="23">
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -1385,16 +1475,43 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment wrapText="1"/>
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1422,6 +1539,10 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[3_Findings_Tables_&amp;_Graphs.xlsx]q1!PivotTable5</c:name>
+    <c:fmtId val="2"/>
+  </c:pivotSource>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1443,22 +1564,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>Maize</a:t>
+              <a:rPr lang="en-US" sz="1200" b="1"/>
+              <a:t>Traits that farmers consider when choosing a variety to grow</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" baseline="0"/>
-              <a:t> t</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>raits that</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" baseline="0"/>
-              <a:t> farmers consider important when choosing a variety to grow</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1100"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1492,6 +1600,64 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1501,6 +1667,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'q1'!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1511,44 +1688,186 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>'q1'!$G$21:$G$23</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Production-related traits</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Consuption-related traits</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Both production &amp; consumption traits</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>'q1'!$G$4:$H$22</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Flour expansion after cooking</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Nutrition/protein</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Maturity time</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Shelf life</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Quality of flour (color &amp; texture)</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Palatability (sweet &amp; smooth taste)</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Milling out-turn</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Grain size/weight</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Recycling potential</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Cost of seed</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Reqires less inputs</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Pest &amp; disease tolerance</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Drought tolerace</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Yield</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Maturity time</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Consumption</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Production</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Production &amp; consumption</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'q1'!$H$21:$H$23</c:f>
+              <c:f>'q1'!$I$4:$I$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.2820512820512819</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.2820512820512819</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.5641025641025639</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8461538461538458</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4871794871794872</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.6923076923076925</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.256410256410255</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.538461538461538</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2820512820512819</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.4871794871794872</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.1282051282051277</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.3333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.897435897435896</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.102564102564102</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.820512820512819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3254-4B4A-888A-D23B9A33B4CF}"/>
+              <c16:uniqueId val="{00000000-404A-42CB-9D69-AC997C072FBA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1562,11 +1881,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="575175136"/>
-        <c:axId val="575175496"/>
+        <c:axId val="975843296"/>
+        <c:axId val="975844016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="575175136"/>
+        <c:axId val="975843296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1609,7 +1928,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="575175496"/>
+        <c:crossAx val="975844016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1617,7 +1936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="575175496"/>
+        <c:axId val="975844016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,6 +1956,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>%</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of responses</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1668,10 +2047,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="575175136"/>
+        <c:crossAx val="975843296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:minorUnit val="1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1683,6 +2061,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1715,6 +2100,21 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
 </c:chartSpace>
 </file>
 
@@ -6052,22 +6452,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>939800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F069CDD-633F-1FCD-3986-0F0650F7D048}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A30B8F67-0EAE-F7C3-A4EC-03523337DD97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6174,16 +6574,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1987550</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>352425</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>149225</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2101850</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6257,52 +6657,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Administrator" refreshedDate="45041.64801597222" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="47" xr:uid="{FF792409-84D8-49D8-B4FA-E01D68E1C7FA}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="B3:E50" sheet="q1"/>
-  </cacheSource>
-  <cacheFields count="4">
-    <cacheField name="Attribute category" numFmtId="0">
-      <sharedItems count="3">
-        <s v="Production"/>
-        <s v="Consumption"/>
-        <s v="Production &amp; consumption"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="attribute" numFmtId="0">
-      <sharedItems count="14">
-        <s v="Yield"/>
-        <s v="Drought tolerace"/>
-        <s v="Grain size/weight"/>
-        <s v="Quality of flour (color &amp; texture)"/>
-        <s v="Milling out-turn"/>
-        <s v="Pest &amp; disease tolerance"/>
-        <s v="Maturity time"/>
-        <s v="Palatability (sweet &amp; smooth taste)"/>
-        <s v="Shelf life"/>
-        <s v="Recycling potential"/>
-        <s v="Nutrition/protein"/>
-        <s v="Flour expansion after cooking"/>
-        <s v="Reqires less inputs"/>
-        <s v="Cost of seed"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number of respondents in the group" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="4"/>
-    </cacheField>
-    <cacheField name="Proportion (%) of responses" numFmtId="2">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.2820512820512819" maxValue="2.5641025641025639"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Administrator" refreshedDate="45041.813186921296" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="29" xr:uid="{8B4B93B9-394C-4279-93B9-321B69F3FE26}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B3:D32" sheet="q7"/>
@@ -6338,7 +6692,7 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Administrator" refreshedDate="45041.815444791668" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="29" xr:uid="{FE7C4F07-AC62-4DFF-9BDF-332B672BCFC8}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B3:E32" sheet="q7"/>
@@ -6393,7 +6747,7 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Administrator" refreshedDate="45041.869189004632" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="14" xr:uid="{7D152035-3DDA-4E73-A626-72CD6878C2CF}">
   <cacheSource type="worksheet">
     <worksheetSource ref="C4:F18" sheet="q6"/>
@@ -6427,7 +6781,7 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Administrator" refreshedDate="45041.874758101854" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="10" xr:uid="{CDE74195-3AC1-4956-8572-2D88B39BBF9A}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B3:E13" sheet="q8"/>
@@ -6461,7 +6815,7 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Administrator" refreshedDate="45045.927777777775" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="17" xr:uid="{3E382416-3F4A-4B68-BF24-7520DCAF1AA9}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B3:D20" sheet="q3"/>
@@ -6492,7 +6846,626 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Administrator" refreshedDate="45050.788346643516" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="47" xr:uid="{BA33C54A-EC7C-4EF3-B356-6FE5EE5EDFFE}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B3:E50" sheet="q1"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Attribute category" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Production"/>
+        <s v="Consumption"/>
+        <s v="Production &amp; consumption"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="attribute" numFmtId="0">
+      <sharedItems count="14">
+        <s v="Yield"/>
+        <s v="Drought tolerace"/>
+        <s v="Grain size/weight"/>
+        <s v="Quality of flour (color &amp; texture)"/>
+        <s v="Milling out-turn"/>
+        <s v="Pest &amp; disease tolerance"/>
+        <s v="Maturity time"/>
+        <s v="Palatability (sweet &amp; smooth taste)"/>
+        <s v="Shelf life"/>
+        <s v="Recycling potential"/>
+        <s v="Nutrition/protein"/>
+        <s v="Flour expansion after cooking"/>
+        <s v="Reqires less inputs"/>
+        <s v="Cost of seed"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number of respondents in the group" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="4"/>
+    </cacheField>
+    <cacheField name="Proportion (%) of responses" numFmtId="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.2820512820512819" maxValue="2.5641025641025639"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="29">
+  <r>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="1.7391304347826086"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2"/>
+    <n v="1.7391304347826086"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2"/>
+    <n v="1.7391304347826086"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="2"/>
+    <n v="1.7391304347826086"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2"/>
+    <n v="1.7391304347826086"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="29">
+  <r>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="4"/>
+    <n v="3.4782608695652173"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="1.7391304347826086"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2"/>
+    <n v="1.7391304347826086"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2"/>
+    <n v="1.7391304347826086"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="2"/>
+    <n v="1.7391304347826086"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2"/>
+    <n v="1.7391304347826086"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="5.2173913043478262"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3"/>
+    <n v="2.6086956521739131"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="14">
+  <r>
+    <x v="0"/>
+    <s v="Flour from some varities like Bazooka is more white"/>
+    <n v="3"/>
+    <n v="6.666666666666667"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Some varieties like Bazooka are sweeter"/>
+    <n v="3"/>
+    <n v="6.666666666666667"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Some varieties like Bazooka produce bigger/heavier grains"/>
+    <n v="3"/>
+    <n v="6.666666666666667"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Some varieties are Longe 5 and Longe 10H whiter"/>
+    <n v="4"/>
+    <n v="8.8888888888888893"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Some varieties like landraces, Longe 5 and Longe H614 are sweeter"/>
+    <n v="4"/>
+    <n v="8.8888888888888893"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Landraces have a red cob"/>
+    <n v="4"/>
+    <n v="8.8888888888888893"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Local varieties are sweeter than improved varieties"/>
+    <n v="4"/>
+    <n v="8.8888888888888893"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Improved varieties are whiter than local varieties"/>
+    <n v="4"/>
+    <n v="8.8888888888888893"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Improved varieties take less time to get ready"/>
+    <n v="4"/>
+    <n v="8.8888888888888893"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Hybrib varieties produce more maize floor than local varieities"/>
+    <n v="3"/>
+    <n v="6.666666666666667"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Roasted local varieties are sweeter than hybrids"/>
+    <n v="3"/>
+    <n v="6.666666666666667"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Some varieties like Bazooka are sweeter"/>
+    <n v="2"/>
+    <n v="4.4444444444444446"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="E.g Longe 5 has a smaller grain coating"/>
+    <n v="2"/>
+    <n v="4.4444444444444446"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="E.G Longe 4 has very samm grains"/>
+    <n v="2"/>
+    <n v="4.4444444444444446"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="10">
+  <r>
+    <x v="0"/>
+    <s v="."/>
+    <n v="3"/>
+    <n v="8.5714285714285712"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="."/>
+    <n v="3"/>
+    <n v="8.5714285714285712"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="."/>
+    <n v="3"/>
+    <n v="8.5714285714285712"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="."/>
+    <n v="4"/>
+    <n v="11.428571428571429"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="."/>
+    <n v="4"/>
+    <n v="11.428571428571429"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="."/>
+    <n v="4"/>
+    <n v="11.428571428571429"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="."/>
+    <n v="4"/>
+    <n v="11.428571428571429"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="."/>
+    <n v="4"/>
+    <n v="11.428571428571429"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="."/>
+    <n v="3"/>
+    <n v="8.5714285714285712"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="."/>
+    <n v="3"/>
+    <n v="8.5714285714285712"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="17">
+  <r>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="4"/>
+    <n v="7.0175438596491224"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="5.2631578947368416"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="5.2631578947368416"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="3"/>
+    <n v="5.2631578947368416"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2"/>
+    <n v="3.5087719298245612"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="3.5087719298245612"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="3.5087719298245612"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2"/>
+    <n v="3.5087719298245612"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="47">
   <r>
     <x v="0"/>
@@ -6779,592 +7752,20 @@
 </pivotCacheRecords>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="29">
-  <r>
-    <x v="0"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="2"/>
-    <n v="1.7391304347826086"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="2"/>
-    <n v="1.7391304347826086"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <n v="2"/>
-    <n v="1.7391304347826086"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <n v="2"/>
-    <n v="1.7391304347826086"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="2"/>
-    <n v="1.7391304347826086"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="29">
-  <r>
-    <x v="0"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="4"/>
-    <n v="3.4782608695652173"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="2"/>
-    <n v="1.7391304347826086"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="2"/>
-    <n v="1.7391304347826086"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <n v="2"/>
-    <n v="1.7391304347826086"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <n v="2"/>
-    <n v="1.7391304347826086"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="2"/>
-    <n v="1.7391304347826086"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="6"/>
-    <n v="5.2173913043478262"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <n v="3"/>
-    <n v="2.6086956521739131"/>
-    <x v="0"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="14">
-  <r>
-    <x v="0"/>
-    <s v="Flour from some varities like Bazooka is more white"/>
-    <n v="3"/>
-    <n v="6.666666666666667"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <s v="Some varieties like Bazooka are sweeter"/>
-    <n v="3"/>
-    <n v="6.666666666666667"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="Some varieties like Bazooka produce bigger/heavier grains"/>
-    <n v="3"/>
-    <n v="6.666666666666667"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="Some varieties are Longe 5 and Longe 10H whiter"/>
-    <n v="4"/>
-    <n v="8.8888888888888893"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <s v="Some varieties like landraces, Longe 5 and Longe H614 are sweeter"/>
-    <n v="4"/>
-    <n v="8.8888888888888893"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="Landraces have a red cob"/>
-    <n v="4"/>
-    <n v="8.8888888888888893"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <s v="Local varieties are sweeter than improved varieties"/>
-    <n v="4"/>
-    <n v="8.8888888888888893"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="Improved varieties are whiter than local varieties"/>
-    <n v="4"/>
-    <n v="8.8888888888888893"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <s v="Improved varieties take less time to get ready"/>
-    <n v="4"/>
-    <n v="8.8888888888888893"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <s v="Hybrib varieties produce more maize floor than local varieities"/>
-    <n v="3"/>
-    <n v="6.666666666666667"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <s v="Roasted local varieties are sweeter than hybrids"/>
-    <n v="3"/>
-    <n v="6.666666666666667"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <s v="Some varieties like Bazooka are sweeter"/>
-    <n v="2"/>
-    <n v="4.4444444444444446"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <s v="E.g Longe 5 has a smaller grain coating"/>
-    <n v="2"/>
-    <n v="4.4444444444444446"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="E.G Longe 4 has very samm grains"/>
-    <n v="2"/>
-    <n v="4.4444444444444446"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="10">
-  <r>
-    <x v="0"/>
-    <s v="."/>
-    <n v="3"/>
-    <n v="8.5714285714285712"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <s v="."/>
-    <n v="3"/>
-    <n v="8.5714285714285712"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="."/>
-    <n v="3"/>
-    <n v="8.5714285714285712"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="."/>
-    <n v="4"/>
-    <n v="11.428571428571429"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <s v="."/>
-    <n v="4"/>
-    <n v="11.428571428571429"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <s v="."/>
-    <n v="4"/>
-    <n v="11.428571428571429"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <s v="."/>
-    <n v="4"/>
-    <n v="11.428571428571429"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <s v="."/>
-    <n v="4"/>
-    <n v="11.428571428571429"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <s v="."/>
-    <n v="3"/>
-    <n v="8.5714285714285712"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="."/>
-    <n v="3"/>
-    <n v="8.5714285714285712"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="17">
-  <r>
-    <x v="0"/>
-    <n v="4"/>
-    <n v="7.0175438596491224"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="4"/>
-    <n v="7.0175438596491224"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="4"/>
-    <n v="7.0175438596491224"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="4"/>
-    <n v="7.0175438596491224"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="4"/>
-    <n v="7.0175438596491224"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="4"/>
-    <n v="7.0175438596491224"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="4"/>
-    <n v="7.0175438596491224"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="4"/>
-    <n v="7.0175438596491224"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="4"/>
-    <n v="7.0175438596491224"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="4"/>
-    <n v="7.0175438596491224"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="3"/>
-    <n v="5.2631578947368416"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="3"/>
-    <n v="5.2631578947368416"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="3"/>
-    <n v="5.2631578947368416"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="2"/>
-    <n v="3.5087719298245612"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="2"/>
-    <n v="3.5087719298245612"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="2"/>
-    <n v="3.5087719298245612"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="2"/>
-    <n v="3.5087719298245612"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1EB29193-974F-472C-88A7-4CC1BDC915E4}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="G3:H18" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9BAF2BC0-D1C7-417D-899D-D5927A51F939}" name="PivotTable5" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
+  <location ref="G3:I22" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="3">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="4">
         <item x="1"/>
         <item x="0"/>
         <item x="2"/>
+        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="14">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending">
+      <items count="15">
         <item x="13"/>
         <item x="1"/>
         <item x="11"/>
@@ -7379,96 +7780,282 @@
         <item x="12"/>
         <item x="8"/>
         <item x="0"/>
+        <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="2" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="2" outline="0" showAll="0"/>
   </pivotFields>
   <rowFields count="2">
     <field x="0"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="15">
+  <rowItems count="19">
     <i>
       <x/>
       <x v="2"/>
     </i>
     <i r="1">
-      <x v="3"/>
+      <x v="6"/>
     </i>
     <i r="1">
       <x v="4"/>
     </i>
     <i r="1">
-      <x v="5"/>
+      <x v="12"/>
     </i>
     <i r="1">
-      <x v="6"/>
+      <x v="9"/>
     </i>
     <i r="1">
       <x v="7"/>
     </i>
     <i r="1">
-      <x v="9"/>
+      <x v="5"/>
     </i>
     <i r="1">
-      <x v="12"/>
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x/>
     </i>
     <i>
       <x v="1"/>
+      <x v="10"/>
+    </i>
+    <i r="1">
       <x/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
     </i>
     <i r="1">
       <x v="1"/>
     </i>
     <i r="1">
-      <x v="8"/>
+      <x v="13"/>
     </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
+    <i t="default">
+      <x v="1"/>
     </i>
     <i>
       <x v="2"/>
       <x v="4"/>
     </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
-  <formats count="4">
+  <dataFields count="1">
+    <dataField name="Sum of Proportion (%) of responses" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="13">
+    <format dxfId="22">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="8">
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="9"/>
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="8"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="8">
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="9"/>
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="13">
-      <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="8"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
     <format dxfId="12">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
     <format dxfId="11">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
     <format dxfId="10">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
+  <chartFormats count="2">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E675071-7F9E-4464-9AE0-05F19B533BF5}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="14">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E675071-7F9E-4464-9AE0-05F19B533BF5}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="14">
   <location ref="F3:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -7565,7 +8152,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EBADF12C-F5D6-4898-80AD-826B5D8825DD}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EBADF12C-F5D6-4898-80AD-826B5D8825DD}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="10">
   <location ref="H4:I10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -7655,7 +8242,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD7B56AD-6965-4F2A-A066-26CE81EAEFCC}" name="PivotTable12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD7B56AD-6965-4F2A-A066-26CE81EAEFCC}" name="PivotTable12" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
   <location ref="G3:H14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending">
@@ -7784,7 +8371,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43900DDE-4AE8-4A74-9C83-721BACE09DFD}" name="PivotTable13" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43900DDE-4AE8-4A74-9C83-721BACE09DFD}" name="PivotTable13" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="J3:K22" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -7914,7 +8501,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C166D0B-B9FC-4007-A373-7A63ACD9AB31}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C166D0B-B9FC-4007-A373-7A63ACD9AB31}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="4">
   <location ref="G3:H9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -8310,11 +8897,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8325,9 +8912,9 @@
     <col min="4" max="4" width="11.7265625" customWidth="1"/>
     <col min="5" max="5" width="10.90625" customWidth="1"/>
     <col min="6" max="6" width="4.453125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="25.54296875" customWidth="1"/>
+    <col min="7" max="7" width="28.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6328125" customWidth="1"/>
+    <col min="9" max="9" width="19.6328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.36328125" style="11" customWidth="1"/>
     <col min="11" max="11" width="30.1796875" customWidth="1"/>
     <col min="12" max="12" width="8.26953125" customWidth="1"/>
@@ -8367,7 +8954,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="25" t="s">
@@ -8376,16 +8963,18 @@
       <c r="H3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I3"/>
+      <c r="I3" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="J3" s="31"/>
       <c r="K3" s="27" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="L3" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M3" s="28" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -8411,15 +9000,18 @@
       <c r="H4" t="s">
         <v>39</v>
       </c>
+      <c r="I4" s="24">
+        <v>1.2820512820512819</v>
+      </c>
       <c r="K4" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="L4" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -8440,19 +9032,22 @@
         <v>1.9230769230769231</v>
       </c>
       <c r="H5" t="s">
-        <v>144</v>
+        <v>21</v>
+      </c>
+      <c r="I5" s="24">
+        <v>1.2820512820512819</v>
       </c>
       <c r="K5" t="s">
         <v>144</v>
       </c>
       <c r="L5" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M5" s="24">
         <v>11.538461538461538</v>
       </c>
       <c r="N5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -8475,17 +9070,20 @@
       <c r="H6" t="s">
         <v>32</v>
       </c>
+      <c r="I6" s="24">
+        <v>2.5641025641025639</v>
+      </c>
       <c r="K6" t="s">
         <v>33</v>
       </c>
       <c r="L6" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M6" s="24">
         <v>10.256410256410255</v>
       </c>
       <c r="N6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -8506,19 +9104,22 @@
         <v>2.5641025641025639</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="I7" s="24">
+        <v>3.8461538461538458</v>
       </c>
       <c r="K7" t="s">
         <v>38</v>
       </c>
       <c r="L7" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M7" s="24">
         <v>7.6923076923076925</v>
       </c>
       <c r="N7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -8539,19 +9140,22 @@
         <v>2.5641025641025639</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>64</v>
+      </c>
+      <c r="I8" s="24">
+        <v>4.4871794871794872</v>
       </c>
       <c r="K8" t="s">
         <v>64</v>
       </c>
       <c r="L8" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M8" s="24">
         <v>4.4871794871794872</v>
       </c>
       <c r="N8" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -8574,17 +9178,20 @@
       <c r="H9" t="s">
         <v>38</v>
       </c>
+      <c r="I9" s="24">
+        <v>7.6923076923076925</v>
+      </c>
       <c r="K9" t="s">
         <v>31</v>
       </c>
       <c r="L9" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M9" s="24">
         <v>3.8461538461538458</v>
       </c>
       <c r="N9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -8605,19 +9212,22 @@
         <v>2.5641025641025639</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>33</v>
+      </c>
+      <c r="I10" s="24">
+        <v>10.256410256410255</v>
       </c>
       <c r="K10" t="s">
         <v>32</v>
       </c>
       <c r="L10" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M10" s="24">
         <v>2.5641025641025639</v>
       </c>
       <c r="N10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -8638,19 +9248,22 @@
         <v>2.5641025641025639</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>144</v>
+      </c>
+      <c r="I11" s="24">
+        <v>11.538461538461538</v>
       </c>
       <c r="K11" t="s">
         <v>39</v>
       </c>
       <c r="L11" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M11" s="24">
         <v>1.2820512820512819</v>
       </c>
       <c r="N11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -8671,22 +9284,22 @@
         <v>2.5641025641025639</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" t="s">
-        <v>42</v>
+        <v>220</v>
+      </c>
+      <c r="I12" s="24">
+        <v>42.948717948717949</v>
       </c>
       <c r="K12" t="s">
         <v>21</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M12" s="24">
         <v>1.2820512820512819</v>
       </c>
       <c r="N12" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -8706,21 +9319,27 @@
         <f t="shared" si="0"/>
         <v>2.5641025641025639</v>
       </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
       <c r="H13" t="s">
-        <v>28</v>
+        <v>34</v>
+      </c>
+      <c r="I13" s="24">
+        <v>1.2820512820512819</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="L13" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M13" s="24">
         <f>SUM(M5:M12)</f>
         <v>42.948717948717956</v>
       </c>
       <c r="N13" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -8741,17 +9360,20 @@
         <v>2.5641025641025639</v>
       </c>
       <c r="H14" t="s">
-        <v>30</v>
+        <v>42</v>
+      </c>
+      <c r="I14" s="24">
+        <v>4.4871794871794872</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="L14" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M14" s="24"/>
       <c r="N14" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -8772,19 +9394,22 @@
         <v>2.5641025641025639</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>41</v>
+      </c>
+      <c r="I15" s="24">
+        <v>5.1282051282051277</v>
       </c>
       <c r="K15" t="s">
         <v>27</v>
       </c>
       <c r="L15" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M15" s="24">
         <v>14.102564102564102</v>
       </c>
       <c r="N15" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -8805,19 +9430,22 @@
         <v>2.5641025641025639</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>30</v>
+      </c>
+      <c r="I16" s="24">
+        <v>8.3333333333333321</v>
       </c>
       <c r="K16" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M16" s="24">
         <v>10.897435897435896</v>
       </c>
       <c r="N16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -8838,19 +9466,22 @@
         <v>2.5641025641025639</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="I17" s="24">
+        <v>10.897435897435896</v>
       </c>
       <c r="K17" t="s">
         <v>30</v>
       </c>
       <c r="L17" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M17" s="24">
         <v>8.3333333333333321</v>
       </c>
       <c r="N17" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -8870,23 +9501,23 @@
         <f t="shared" si="0"/>
         <v>2.5641025641025639</v>
       </c>
-      <c r="G18" t="s">
-        <v>65</v>
-      </c>
       <c r="H18" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="I18" s="24">
+        <v>14.102564102564102</v>
       </c>
       <c r="K18" t="s">
         <v>41</v>
       </c>
       <c r="L18" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M18" s="24">
         <v>5.1282051282051277</v>
       </c>
       <c r="N18" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -8906,17 +9537,23 @@
         <f t="shared" si="0"/>
         <v>1.9230769230769231</v>
       </c>
+      <c r="G19" t="s">
+        <v>221</v>
+      </c>
+      <c r="I19" s="24">
+        <v>44.230769230769226</v>
+      </c>
       <c r="K19" t="s">
         <v>42</v>
       </c>
       <c r="L19" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M19" s="24">
         <v>4.4871794871794872</v>
       </c>
       <c r="N19" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -8936,20 +9573,26 @@
         <f t="shared" si="0"/>
         <v>1.9230769230769231</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>180</v>
+      <c r="G20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="24">
+        <v>12.820512820512819</v>
       </c>
       <c r="K20" t="s">
         <v>34</v>
       </c>
       <c r="L20" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M20" s="24">
         <v>1.2820512820512819</v>
       </c>
       <c r="N20" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
@@ -8970,24 +9613,23 @@
         <v>1.9230769230769231</v>
       </c>
       <c r="G21" t="s">
-        <v>182</v>
-      </c>
-      <c r="H21" s="23">
-        <f>SUM(I12:I17)</f>
-        <v>0</v>
+        <v>222</v>
+      </c>
+      <c r="I21" s="24">
+        <v>12.820512820512819</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="L21" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M21" s="24">
         <f>SUM(M15:M20)</f>
         <v>44.230769230769226</v>
       </c>
       <c r="N21" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
@@ -9008,21 +9650,20 @@
         <v>1.9230769230769231</v>
       </c>
       <c r="G22" t="s">
-        <v>181</v>
-      </c>
-      <c r="H22" s="23">
-        <f>SUM(I4:I11)</f>
-        <v>0</v>
+        <v>188</v>
+      </c>
+      <c r="I22">
+        <v>100</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L22" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M22" s="24"/>
       <c r="N22" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
@@ -9042,24 +9683,19 @@
         <f t="shared" si="0"/>
         <v>1.9230769230769231</v>
       </c>
-      <c r="G23" t="s">
-        <v>183</v>
-      </c>
-      <c r="H23" s="23" t="e">
-        <f>GETPIVOTDATA("Proportion (%) of responses",$G$3,"Attribute category","Production &amp; consumption","attribute","Maturity time")</f>
-        <v>#REF!</v>
-      </c>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
       <c r="K23" s="29" t="s">
         <v>32</v>
       </c>
       <c r="L23" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M23" s="30">
         <v>12.820512820512819</v>
       </c>
       <c r="N23" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
@@ -9080,17 +9716,17 @@
         <v>1.2820512820512819</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="L24" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M24" s="24">
         <f>SUM(M23)</f>
         <v>12.820512820512819</v>
       </c>
       <c r="N24" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
@@ -9572,9 +10208,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G21:H23">
-    <sortCondition ref="H21:H23"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
   <drawing r:id="rId3"/>
@@ -9621,13 +10254,13 @@
         <v>24</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G3" s="25" t="s">
         <v>166</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="I3"/>
     </row>
@@ -10050,6 +10683,275 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF600919-3001-4E20-9905-483317F92FAF}">
+  <dimension ref="A2:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" s="41">
+        <v>3</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="41">
+        <v>14</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="41">
+        <v>7</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="41">
+        <v>3</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="38" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="41">
+        <v>1</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="37"/>
+      <c r="B8" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E8" s="41">
+        <v>4</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9" s="41">
+        <v>1</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="37"/>
+      <c r="B10" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" s="41">
+        <v>3</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" s="42">
+        <f>SUM(E3:E10)</f>
+        <v>36</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" s="42">
+        <f>E3+E5+E8+E10</f>
+        <v>17</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="G12" s="23">
+        <f>E12/E11</f>
+        <v>0.47222222222222221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" s="42">
+        <f>E11-E12</f>
+        <v>19</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="G13" s="23">
+        <f>E13/E11</f>
+        <v>0.52777777777777779</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{21FA4ACC-F7F0-4F6E-8C93-03D43C56C784}"/>
+    <hyperlink ref="F3:F13" r:id="rId2" display="\\" xr:uid="{4568A06A-437E-409E-B93D-DB3B7256D100}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I19"/>
@@ -10071,11 +10973,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
       <c r="E1" s="16" t="s">
         <v>83</v>
       </c>
@@ -10511,13 +11413,13 @@
         <v>24</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H3"/>
     </row>
@@ -10662,7 +11564,7 @@
         <v>7.0175438596491224</v>
       </c>
       <c r="F10" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G10">
         <v>100</v>
@@ -11222,13 +12124,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -11251,13 +12153,13 @@
         <v>24</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="H4" s="25" t="s">
         <v>138</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J4"/>
     </row>
@@ -11614,8 +12516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E8F723-8302-46E0-80A7-A4B507221238}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
@@ -11642,21 +12544,21 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="G2" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="H2" s="39"/>
-      <c r="J2" s="40" t="s">
-        <v>191</v>
-      </c>
-      <c r="K2" s="40"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="G2" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="H2" s="45"/>
+      <c r="J2" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="1:12" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
@@ -11669,7 +12571,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>63</v>
@@ -11679,7 +12581,7 @@
         <v>22</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="25" t="s">
@@ -12604,19 +13506,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFECC893-9DC8-4F98-A754-8DFA5B5BA96D}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A2" sqref="A2:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.36328125" customWidth="1"/>
+    <col min="2" max="2" width="2.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.36328125" customWidth="1"/>
-    <col min="5" max="5" width="78.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -12624,19 +13526,19 @@
         <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -12644,229 +13546,304 @@
         <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C2" s="24">
         <v>29.565217391304351</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="F2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>144</v>
-      </c>
       <c r="B3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" s="24">
-        <v>14.782608695652174</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="C3" s="24"/>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>208</v>
       </c>
       <c r="F3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
       <c r="B4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C4" s="24">
-        <v>13.913043478260869</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="C4" s="24"/>
       <c r="D4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C5" s="24">
-        <v>11.304347826086957</v>
+        <v>14.782608695652174</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E5" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="F5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C6" s="24">
-        <v>6.0869565217391308</v>
+        <v>13.913043478260869</v>
       </c>
       <c r="D6" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E6" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="F6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
       <c r="B7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C7" s="24">
-        <v>5.2173913043478262</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="C7" s="24"/>
       <c r="D7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E7" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="F7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>179</v>
-      </c>
       <c r="B8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C8" s="24">
-        <v>5.2173913043478262</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="C8" s="24"/>
       <c r="D8" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E8" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="F8" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="24">
+        <v>11.304347826086957</v>
+      </c>
+      <c r="D9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9" t="s">
         <v>194</v>
       </c>
-      <c r="C9" s="24">
-        <v>5.2173913043478262</v>
-      </c>
-      <c r="D9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E9" t="s">
-        <v>202</v>
-      </c>
       <c r="F9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C10" s="24">
-        <v>5.2173913043478262</v>
+        <v>6.0869565217391308</v>
       </c>
       <c r="D10" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E10" t="s">
-        <v>160</v>
+        <v>214</v>
       </c>
       <c r="F10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="24">
+        <v>5.2173913043478262</v>
+      </c>
+      <c r="D11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" t="s">
+        <v>216</v>
+      </c>
+      <c r="F12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="24">
+        <v>5.2173913043478262</v>
+      </c>
+      <c r="D13" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" t="s">
+        <v>194</v>
+      </c>
+      <c r="F13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="24">
+        <v>5.2173913043478262</v>
+      </c>
+      <c r="D14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14" t="s">
+        <v>194</v>
+      </c>
+      <c r="F14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="24">
+        <v>5.2173913043478262</v>
+      </c>
+      <c r="D15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C11" s="24">
+      <c r="B16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C16" s="24">
         <v>1.7391304347826086</v>
       </c>
-      <c r="D11" t="s">
-        <v>194</v>
-      </c>
-      <c r="E11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="D16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" t="s">
+        <v>218</v>
+      </c>
+      <c r="F16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
-        <v>194</v>
-      </c>
-      <c r="C12" s="24">
+      <c r="B17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" s="24">
         <v>1.7391304347826086</v>
       </c>
-      <c r="D12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" t="s">
-        <v>195</v>
+      <c r="D17" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" t="s">
+        <v>219</v>
+      </c>
+      <c r="F17" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
-    <sortCondition descending="1" ref="C2:C12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E17">
+    <sortCondition descending="1" ref="C2:C17"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" xr:uid="{23A77438-92D4-457D-9A79-DCABFC1E3A86}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{36AFC6C0-8CC7-4E71-9E7E-15D562A308EC}"/>
-    <hyperlink ref="F3:F12" r:id="rId3" display="\\" xr:uid="{36A3B0C4-989F-4A72-BD05-CE208A32A965}"/>
+    <hyperlink ref="F3:F17" r:id="rId3" display="\\" xr:uid="{9119165B-F60A-475D-97D5-7194C4FB8887}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
@@ -12914,7 +13891,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>